<commit_message>
Update Sushi config 81807958f4922eb200d80c10c42b07cc18f0f90c
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-CSCommunicationModes.xlsx
+++ b/main/ig/CodeSystem-CSCommunicationModes.xlsx
@@ -60,13 +60,13 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-27T14:50:30+00:00</t>
+    <t>2024-03-29T13:41:33+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
   </si>
   <si>
-    <t>DOMASIA team of the Signal and Image Processing Laboratory (LTSI)</t>
+    <t>DOMASIA team of the Signal and Image Processing Laboratory (LTSI) and KEREVAL</t>
   </si>
   <si>
     <t>Contact</t>

</xml_diff>

<commit_message>
update profile and add extensions for medication item provenance and events b56dcce53f54dbd3e89fcd2aff1dadf3ca8fd7f1
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-CSCommunicationModes.xlsx
+++ b/main/ig/CodeSystem-CSCommunicationModes.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-18T13:54:15+00:00</t>
+    <t>2024-06-11T08:08:31+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>CodeSystem for french communication modes (incremental, summary).</t>
+    <t>CodeSystem for french communication modes (Incrémental, Récapitulatif).</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -135,13 +135,13 @@
     <t>I</t>
   </si>
   <si>
-    <t>Incremental</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Summary</t>
+    <t>Incrémental</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Récapitulatif</t>
   </si>
 </sst>
 </file>

</xml_diff>